<commit_message>
tansform data before other transformations
</commit_message>
<xml_diff>
--- a/test/fixtures/file-with-tabs/input.xlsx
+++ b/test/fixtures/file-with-tabs/input.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Issac Garza'!$C$1:$C$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Issac Garza'!$C$1:$C$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Issac Garza'!$C$1:$C$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t xml:space="preserve">Tracking Id</t>
   </si>
@@ -209,16 +210,14 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,6 +324,9 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>22</v>

</xml_diff>